<commit_message>
Add experience for permissions to the app
</commit_message>
<xml_diff>
--- a/src/Ezac.Roster.Web/wwwroot/templates/template.xlsx
+++ b/src/Ezac.Roster.Web/wwwroot/templates/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siegfried.derdeyn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EF28B3-7027-4A6F-8851-1EBC5440E2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3A72A04-026A-4466-A65B-3588D44C2184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,17 +19,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Leden!$A$1:$G$50</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -56,12 +67,6 @@
   </si>
   <si>
     <t>jan.jansens@fake.ezac.nl</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>Piet Pieters</t>
@@ -428,7 +433,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -763,7 +768,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,17 +809,17 @@
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
+      <c r="C2" s="3">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -822,22 +827,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
         <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -845,22 +850,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -868,22 +873,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -891,22 +896,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
       </c>
       <c r="G6" s="3">
         <v>0.5</v>
@@ -914,22 +919,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8</v>
       </c>
       <c r="G7" s="3">
         <v>0.5</v>
@@ -937,22 +942,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
       </c>
       <c r="G8" s="3">
         <v>0.5</v>
@@ -960,22 +965,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -983,22 +988,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
         <v>9</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>9</v>
+      <c r="F10" s="3">
+        <v>8</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -1006,22 +1011,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -1029,22 +1034,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1052,22 +1057,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1075,22 +1080,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1098,22 +1103,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
         <v>9</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>9</v>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1121,22 +1126,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="C16" s="3">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
@@ -1144,22 +1149,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>9</v>
+        <v>38</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -1167,22 +1172,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4</v>
       </c>
       <c r="G18" s="3">
         <v>0.5</v>
@@ -1190,22 +1195,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3">
         <v>10</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>9</v>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3">
+        <v>6</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
@@ -1213,22 +1218,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
@@ -1236,22 +1241,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8</v>
       </c>
       <c r="G21" s="3">
         <v>0.5</v>
@@ -1259,22 +1264,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
         <v>9</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
+      <c r="F22" s="3">
+        <v>0</v>
       </c>
       <c r="G22" s="3">
         <v>0.5</v>
@@ -1282,22 +1287,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>6</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>7</v>
       </c>
       <c r="G23" s="3">
         <v>1</v>
@@ -1305,22 +1310,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -1328,22 +1333,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>10</v>
+        <v>54</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
@@ -1351,22 +1356,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>2</v>
       </c>
       <c r="G26" s="3">
         <v>1</v>
@@ -1374,22 +1379,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
         <v>10</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="3">
         <v>10</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
       </c>
       <c r="G27" s="3">
         <v>1</v>
@@ -1397,22 +1402,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>9</v>
+        <v>60</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>4</v>
       </c>
       <c r="G28" s="3">
         <v>1</v>
@@ -1420,22 +1425,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>10</v>
+        <v>62</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
       </c>
       <c r="G29" s="3">
         <v>1</v>
@@ -1443,22 +1448,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
         <v>9</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>9</v>
+      <c r="F30" s="3">
+        <v>7</v>
       </c>
       <c r="G30" s="3">
         <v>1</v>
@@ -1466,22 +1471,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>8</v>
+      </c>
+      <c r="F31" s="3">
         <v>10</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="G31" s="3">
         <v>1</v>
@@ -1489,22 +1494,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>9</v>
+        <v>68</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>4</v>
       </c>
       <c r="G32" s="3">
         <v>1</v>
@@ -1512,22 +1517,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>10</v>
+        <v>70</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
       </c>
       <c r="G33" s="3">
         <v>1</v>
@@ -1535,22 +1540,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>9</v>
+        <v>72</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3">
+        <v>6</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
       </c>
       <c r="G34" s="3">
         <v>1</v>
@@ -1558,21 +1563,21 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="3">
+        <v>7</v>
+      </c>
+      <c r="D35" s="3">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3">
+        <v>6</v>
+      </c>
+      <c r="F35" s="3">
         <v>9</v>
       </c>
       <c r="G35" s="3">
@@ -1581,22 +1586,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>10</v>
+        <v>76</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
       </c>
       <c r="G36" s="3">
         <v>1</v>
@@ -1604,22 +1609,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
       </c>
       <c r="G37" s="3">
         <v>0.5</v>
@@ -1627,22 +1632,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>10</v>
+        <v>80</v>
+      </c>
+      <c r="C38" s="3">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>5</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
       </c>
       <c r="G38" s="3">
         <v>1</v>
@@ -1650,22 +1655,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>9</v>
+        <v>82</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>7</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>3</v>
       </c>
       <c r="G39" s="3">
         <v>1</v>
@@ -1673,22 +1678,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>10</v>
+        <v>84</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>6</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
       </c>
       <c r="G40" s="3">
         <v>1</v>
@@ -1696,22 +1701,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="3">
+        <v>6</v>
+      </c>
+      <c r="D41" s="3">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3">
         <v>9</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>9</v>
+      <c r="F41" s="3">
+        <v>4</v>
       </c>
       <c r="G41" s="3">
         <v>0.5</v>
@@ -1719,22 +1724,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>9</v>
+        <v>88</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>8</v>
       </c>
       <c r="G42" s="3">
         <v>1</v>
@@ -1742,22 +1747,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>10</v>
+        <v>90</v>
+      </c>
+      <c r="C43" s="3">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3">
+        <v>4</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
       </c>
       <c r="G43" s="3">
         <v>1</v>
@@ -1765,22 +1770,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
+      </c>
+      <c r="C44" s="3">
+        <v>3</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>8</v>
+      </c>
+      <c r="F44" s="3">
+        <v>7</v>
       </c>
       <c r="G44" s="3">
         <v>1</v>
@@ -1788,22 +1793,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
         <v>9</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>10</v>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0</v>
       </c>
       <c r="G45" s="3">
         <v>1</v>
@@ -1811,22 +1816,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>9</v>
+        <v>96</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
       </c>
       <c r="G46" s="3">
         <v>1</v>
@@ -1834,22 +1839,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>9</v>
+        <v>98</v>
+      </c>
+      <c r="C47" s="3">
+        <v>3</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
       </c>
       <c r="G47" s="3">
         <v>1</v>
@@ -1857,22 +1862,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
       </c>
       <c r="G48" s="3">
         <v>0</v>
@@ -1880,22 +1885,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>9</v>
+        <v>102</v>
+      </c>
+      <c r="C49" s="3">
+        <v>4</v>
+      </c>
+      <c r="D49" s="3">
+        <v>6</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>7</v>
       </c>
       <c r="G49" s="3">
         <v>0</v>
@@ -1903,22 +1908,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>10</v>
+        <v>104</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>8</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
       </c>
       <c r="G50" s="3">
         <v>1</v>
@@ -1947,17 +1952,17 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2001,12 +2006,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8f2bba8-69e4-46d2-bf76-63856e481934">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2244,20 +2251,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8f2bba8-69e4-46d2-bf76-63856e481934">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{825E5DDC-5EEE-446E-A794-28D40B64AE16}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{391C8BE3-9239-4163-AB5E-F1B248A6E4CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <ds:schemaRef ds:uri="d8f2bba8-69e4-46d2-bf76-63856e481934"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2283,12 +2291,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{391C8BE3-9239-4163-AB5E-F1B248A6E4CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{825E5DDC-5EEE-446E-A794-28D40B64AE16}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <ds:schemaRef ds:uri="d8f2bba8-69e4-46d2-bf76-63856e481934"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>